<commit_message>
[TimesheetCalculatorV2] Changes: * added a test for overnight work (passed 12midnight)
</commit_message>
<xml_diff>
--- a/python_source/Timesheet Calculator v2/Timesheet Calculator v2/test/mvc/testdata/testdata_003.xlsx
+++ b/python_source/Timesheet Calculator v2/Timesheet Calculator v2/test/mvc/testdata/testdata_003.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t xml:space="preserve">PROFESSOR TORSTEN CALVI CORP.</t>
   </si>
@@ -78,6 +78,12 @@
   </si>
   <si>
     <t xml:space="preserve">Project5905</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Task094305</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Project 0910291</t>
   </si>
   <si>
     <t xml:space="preserve">Note: Insert new rows above (right-click &gt; “Insert Rows Above”) for new entry.</t>
@@ -370,15 +376,15 @@
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="28.25"/>
   </cols>
@@ -476,11 +482,21 @@
       <c r="F11" s="4"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="7"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
+      <c r="A12" s="7" t="n">
+        <v>44376</v>
+      </c>
+      <c r="B12" s="8" t="n">
+        <v>0.708333333333333</v>
+      </c>
+      <c r="C12" s="8" t="n">
+        <v>0.0416666666666667</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="F12" s="4"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -509,7 +525,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="9" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B16" s="10"/>
       <c r="C16" s="10"/>
@@ -519,7 +535,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -528,7 +544,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -537,12 +553,12 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B32" s="10"/>
       <c r="C32" s="10"/>
@@ -572,7 +588,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>